<commit_message>
changed course schema and home page
</commit_message>
<xml_diff>
--- a/frontend/public/shablon.xlsx
+++ b/frontend/public/shablon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mssho\OneDrive\Рабочий стол\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\malaka\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C58DD15-A0CA-4D3C-8D50-F46B5FDFF52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A59C8AF-2A4A-4314-9F20-019F9EB461C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,37 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
-  <si>
-    <t>Beridev Baxtiyor Kalonovich</t>
-  </si>
-  <si>
-    <t>Ibragimov Alisher Ulugbekovich</t>
-  </si>
-  <si>
-    <t>Karimov Shavkat Mirziyoevich</t>
-  </si>
-  <si>
-    <t>Nuriddinov Farrux Saidovich</t>
-  </si>
-  <si>
-    <t>Raximov Aziz Baxtiyorovich</t>
-  </si>
-  <si>
-    <t>Saidova Zuxra Abdullaevna</t>
-  </si>
-  <si>
-    <t>Tursunov Djaxongir Rustamovich</t>
-  </si>
-  <si>
-    <t>Umarov Rustam Alisherovich</t>
-  </si>
-  <si>
-    <t>Fayzullaev Alisher Rustamovich</t>
-  </si>
-  <si>
-    <t>Xodjaev Baxtiyor Alisherovich</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>kapitan</t>
   </si>
@@ -73,15 +43,72 @@
   </si>
   <si>
     <t>passport</t>
+  </si>
+  <si>
+    <t>Raximov Zuxra Ulugbekovich</t>
+  </si>
+  <si>
+    <t>57445676413902</t>
+  </si>
+  <si>
+    <t>Tursunov Shavkat Baxtiyorovich</t>
+  </si>
+  <si>
+    <t>59495000621590</t>
+  </si>
+  <si>
+    <t>Umarov Zuxra Abdullaevna</t>
+  </si>
+  <si>
+    <t>98996542501757</t>
+  </si>
+  <si>
+    <t>Nuriddinov Farrux Kalonovich</t>
+  </si>
+  <si>
+    <t>72597068945989</t>
+  </si>
+  <si>
+    <t>Tursunov Baxtiyor Ulugbekovich</t>
+  </si>
+  <si>
+    <t>52682959199863</t>
+  </si>
+  <si>
+    <t>Raximov Said Mirziyoevich</t>
+  </si>
+  <si>
+    <t>65390187330537</t>
+  </si>
+  <si>
+    <t>Ibragimov Baxtiyor Mirziyoevich</t>
+  </si>
+  <si>
+    <t>53318845013302</t>
+  </si>
+  <si>
+    <t>Raximov Aziz Kalonovich</t>
+  </si>
+  <si>
+    <t>11924142676175</t>
+  </si>
+  <si>
+    <t>Tursunov Alisher Djaxongirovich</t>
+  </si>
+  <si>
+    <t>15144815304021</t>
+  </si>
+  <si>
+    <t>Raximov Ulugbek Ulugbekovich</t>
+  </si>
+  <si>
+    <t>24523908669485</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,10 +126,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,20 +150,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{F146F8B7-E5EA-414E-8816-9B746C77883E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -416,7 +441,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,123 +456,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>78658912657851</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>32549865781245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2">
-        <v>87896554212356</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2">
-        <v>12326545788956</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45658978123278</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2">
-        <v>52749685416352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2">
-        <v>10526396857420</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2">
-        <v>89205763418065</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2">
-        <v>78652305194826</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2">
-        <v>78542129578921</v>
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>